<commit_message>
minor updates to iptds website
</commit_message>
<xml_diff>
--- a/data/prioritization/iptds_site_recommendations_20240411.xlsx
+++ b/data/prioritization/iptds_site_recommendations_20240411.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeR_IPTDS\data\derived_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeRiverIPTDS\data\prioritization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9986E97D-ECFD-4D44-BD68-539D29D27C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBBBA8A6-E89B-4B46-AF7F-50BFCE87BDF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="16440" windowHeight="28590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="144">
   <si>
     <t>site_code</t>
   </si>
@@ -213,9 +213,6 @@
     <t>ACM</t>
   </si>
   <si>
-    <t>ALP (Proposed)</t>
-  </si>
-  <si>
     <t>SLT (Proposed)</t>
   </si>
   <si>
@@ -399,12 +396,6 @@
     <t>LOW</t>
   </si>
   <si>
-    <t>USU (Proposed)</t>
-  </si>
-  <si>
-    <t>USI (Proposed)</t>
-  </si>
-  <si>
     <t>MED</t>
   </si>
   <si>
@@ -438,9 +429,6 @@
     <t>Alternative locations: East Fork Salmon River.</t>
   </si>
   <si>
-    <t>Move upstream to proposed USI location.</t>
-  </si>
-  <si>
     <t>Alternate locations: upper Chamberlain, Sabe, Bargamin, Warren, Crooked, or Sheep creeks.</t>
   </si>
   <si>
@@ -453,22 +441,37 @@
     <t>Consider upgrade to IS1001 MC and tandem arrays if sufficient distance btw arrays can be achieved.</t>
   </si>
   <si>
-    <t>One of LAP, JUL, or LAW should be funded to provide monitoring in the CRLMA-s population. LAP or JUL would be preferred to continue time-series of estimates.</t>
-  </si>
-  <si>
     <t>New site could be a single-pass array.</t>
   </si>
   <si>
-    <t>Either LLR or both HYC and LRW could long-term be considered for consolidation to single-pass arrays, especially if sites(s) were upgraded with IS1001 MC(s).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Planned upgrade to IS1001 MC. Alternatively, LLR could be considered for upgrade to IS1001 MC to increase juvenile detections. Either LLR or both HYC and LRW could long-term be considered for consolidation to single-pass arrays, especially if sites(s) were upgraded with IS1001 MC(s).   </t>
-  </si>
-  <si>
     <t>If feasible, SW2 could be moved to the end of the Selway Road which would allow parsing of the SEMOO and SEUMA populations from SEMEA.</t>
   </si>
   <si>
-    <t>Likely not necessary; a weir is operated near the lower 1 rkm of Alpowa Creek and has generated census estimates in nearly all of the previous 19 years.</t>
+    <t>USC (Proposed)</t>
+  </si>
+  <si>
+    <t>USP (Proposed)</t>
+  </si>
+  <si>
+    <t>LLR could be considered for consolidation to a single-pass array, especially if upgraded to a IS1001 MC.</t>
+  </si>
+  <si>
+    <t>Planned upgrade to IS1001 MC.</t>
+  </si>
+  <si>
+    <t>Important site for in-season adult monitoring and juvenile survival monitoring.</t>
+  </si>
+  <si>
+    <t>WB1 (Proposed)</t>
+  </si>
+  <si>
+    <t>If not already, consider upgrade to IS1001 MC to increase read range.</t>
+  </si>
+  <si>
+    <t>Move upstream to proposed USP location.</t>
+  </si>
+  <si>
+    <t>One of LAP or (previous) JUL should be funded to provide monitoring in the CRLMA-s population.</t>
   </si>
 </sst>
 </file>
@@ -811,10 +814,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F54"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52:XFD52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -836,10 +839,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -877,15 +880,15 @@
         <v>-114.72045300000001</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
@@ -897,10 +900,10 @@
         <v>-114.35290000000001</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -917,12 +920,12 @@
         <v>-114.30289999999999</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>8</v>
@@ -934,10 +937,10 @@
         <v>-114.0744</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -954,10 +957,10 @@
         <v>-113.964145</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -974,10 +977,10 @@
         <v>-113.916319</v>
       </c>
       <c r="E8" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -993,9 +996,11 @@
       <c r="D9" s="3">
         <v>-113.885278</v>
       </c>
-      <c r="E9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>117</v>
+      </c>
       <c r="F9" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1012,7 +1017,7 @@
         <v>-113.746897</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -1029,9 +1034,6 @@
         <v>-113.63193699999999</v>
       </c>
       <c r="E11" s="4"/>
-      <c r="F11" s="2" t="s">
-        <v>139</v>
-      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
@@ -1046,11 +1048,9 @@
       <c r="D12" s="3">
         <v>-113.62472099999999</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>121</v>
-      </c>
+      <c r="E12" s="4"/>
       <c r="F12" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1067,7 +1067,7 @@
         <v>-113.545027</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1084,7 +1084,7 @@
         <v>-113.374118</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1101,7 +1101,7 @@
         <v>-113.365281</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1133,10 +1133,10 @@
         <v>-114.358101</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1153,10 +1153,10 @@
         <v>-114.9449</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1203,7 +1203,10 @@
         <v>-115.579712</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -1235,10 +1238,10 @@
         <v>-115.53315000000001</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1255,10 +1258,10 @@
         <v>-115.73302</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1275,15 +1278,15 @@
         <v>-116.3293</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>30</v>
+        <v>140</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>8</v>
@@ -1295,12 +1298,12 @@
         <v>-116.306603</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>8</v>
@@ -1312,7 +1315,7 @@
         <v>-116.2645</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1329,7 +1332,7 @@
         <v>-115.56588600000001</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1346,10 +1349,10 @@
         <v>-115.515533</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1396,10 +1399,10 @@
         <v>-115.981313</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>126</v>
+        <v>141</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1416,10 +1419,10 @@
         <v>-115.97776</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1436,10 +1439,10 @@
         <v>-115.815972</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1456,10 +1459,10 @@
         <v>-115.6341</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1476,7 +1479,7 @@
         <v>-115.52766</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1493,10 +1496,10 @@
         <v>-115.97615999999999</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1513,10 +1516,10 @@
         <v>-115.933747</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1533,10 +1536,10 @@
         <v>-116.812535</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1553,272 +1556,226 @@
         <v>-116.709318</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C41" s="3">
-        <v>46.218468999999999</v>
+        <v>45.761051999999999</v>
       </c>
       <c r="D41" s="3">
-        <v>-116.02898500000001</v>
+        <v>-116.750231</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C42" s="3">
-        <v>45.761051999999999</v>
+        <v>45.742702000000001</v>
       </c>
       <c r="D42" s="3">
-        <v>-116.750231</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>129</v>
-      </c>
+        <v>-116.764304</v>
+      </c>
+      <c r="E42" s="4"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C43" s="3">
-        <v>45.742702000000001</v>
+        <v>45.489956999999997</v>
       </c>
       <c r="D43" s="3">
-        <v>-116.764304</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>118</v>
-      </c>
+        <v>-116.804096</v>
+      </c>
+      <c r="E43" s="4"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C44" s="3">
-        <v>45.489956999999997</v>
+        <v>45.767740000000003</v>
       </c>
       <c r="D44" s="3">
-        <v>-116.804096</v>
+        <v>-116.74403700000001</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C45" s="3">
-        <v>45.767740000000003</v>
+        <v>45.506481999999998</v>
       </c>
       <c r="D45" s="3">
-        <v>-116.74403700000001</v>
+        <v>-116.850735</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C46" s="3">
-        <v>45.506481999999998</v>
+        <v>45.593519999999998</v>
       </c>
       <c r="D46" s="3">
-        <v>-116.850735</v>
+        <v>-117.903379</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>118</v>
       </c>
+      <c r="F46" s="2" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C47" s="3">
-        <v>45.593519999999998</v>
+        <v>45.633679000000001</v>
       </c>
       <c r="D47" s="3">
-        <v>-117.903379</v>
+        <v>-117.733757</v>
       </c>
       <c r="E47" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="F47" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C48" s="3">
-        <v>45.633679000000001</v>
+        <v>45.594465999999997</v>
       </c>
       <c r="D48" s="3">
-        <v>-117.733757</v>
+        <v>-117.579223</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C49" s="3">
-        <v>45.594465999999997</v>
+        <v>45.619622999999997</v>
       </c>
       <c r="D49" s="3">
-        <v>-117.579223</v>
+        <v>-117.72657</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C50" s="3">
-        <v>45.619622999999997</v>
+        <v>45.946151</v>
       </c>
       <c r="D50" s="3">
-        <v>-117.72657</v>
+        <v>-117.45412399999999</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>118</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C51" s="3">
-        <v>45.946151</v>
+        <v>46.030237</v>
       </c>
       <c r="D51" s="3">
-        <v>-117.45412399999999</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>130</v>
-      </c>
+        <v>-117.016408</v>
+      </c>
+      <c r="E51" s="4"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C52" s="3">
-        <v>46.030237</v>
+        <v>46.341368000000003</v>
       </c>
       <c r="D52" s="3">
-        <v>-117.016408</v>
+        <v>-117.055707</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C53" s="3">
-        <v>46.341368000000003</v>
-      </c>
-      <c r="D53" s="3">
-        <v>-117.055707</v>
-      </c>
-      <c r="E53" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C54" s="3">
-        <v>46.4054</v>
-      </c>
-      <c r="D54" s="3">
-        <v>-117.22450000000001</v>
-      </c>
-      <c r="E54" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>142</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1847,15 +1804,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="1">
         <v>46.544192000000002</v>
@@ -1866,7 +1823,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" s="1">
         <v>46.505239000000003</v>
@@ -1877,7 +1834,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" s="1">
         <v>46.415922000000002</v>
@@ -1888,7 +1845,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" s="1">
         <v>46.309626999999999</v>
@@ -1899,7 +1856,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B6" s="1">
         <v>46.204596000000002</v>
@@ -1910,7 +1867,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B7" s="1">
         <v>46.713909000000001</v>
@@ -1932,7 +1889,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B9" s="1">
         <v>46.369216999999999</v>
@@ -1943,7 +1900,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B10" s="1">
         <v>46.325991999999999</v>
@@ -1954,7 +1911,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B11" s="1">
         <v>46.367061999999997</v>
@@ -1976,7 +1933,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B13" s="1">
         <v>46.619115000000001</v>
@@ -1987,7 +1944,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B14" s="1">
         <v>46.627882</v>
@@ -1998,7 +1955,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B15" s="1">
         <v>46.630673000000002</v>
@@ -2009,7 +1966,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B16" s="1">
         <v>46.795090999999999</v>
@@ -2020,7 +1977,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B17" s="1">
         <v>46.799005999999999</v>
@@ -2031,7 +1988,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B18" s="1">
         <v>46.503864</v>
@@ -2064,7 +2021,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B21" s="1">
         <v>46.524406999999997</v>
@@ -2075,7 +2032,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B22" s="1">
         <v>46.301448000000001</v>
@@ -2119,7 +2076,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B26" s="1">
         <v>46.132739000000001</v>
@@ -2218,7 +2175,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B35" s="1">
         <v>46.325583999999999</v>
@@ -2229,7 +2186,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B36" s="1">
         <v>46.288457999999999</v>
@@ -2240,7 +2197,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B37" s="1">
         <v>46.272486999999998</v>
@@ -2306,7 +2263,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B43" s="1">
         <v>45.735104999999997</v>
@@ -2328,7 +2285,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B45">
         <v>45.190964000000001</v>
@@ -2339,7 +2296,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B46" s="1">
         <v>45.215252</v>
@@ -2350,7 +2307,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B47" s="1">
         <v>45.248955000000002</v>
@@ -2405,7 +2362,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B52" s="1">
         <v>44.928995</v>
@@ -2438,7 +2395,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B55" s="1">
         <v>44.427939000000002</v>
@@ -2482,7 +2439,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B59" s="1">
         <v>45.246485</v>
@@ -2504,7 +2461,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B61" s="1">
         <v>45.115074</v>
@@ -2515,7 +2472,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B62" s="1">
         <v>45.113169999999997</v>
@@ -2526,7 +2483,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B63" s="1">
         <v>45.111257000000002</v>
@@ -2537,7 +2494,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B64" s="1">
         <v>45.112769999999998</v>
@@ -2559,7 +2516,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B66" s="1">
         <v>45.109456999999999</v>
@@ -2570,7 +2527,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B67" s="1">
         <v>45.100087000000002</v>
@@ -2581,7 +2538,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B68" s="1">
         <v>45.097937999999999</v>
@@ -2592,7 +2549,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B69" s="1">
         <v>45.026792</v>
@@ -2603,7 +2560,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B70" s="1">
         <v>44.956738999999999</v>
@@ -2614,7 +2571,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B71" s="1">
         <v>44.896909999999998</v>
@@ -2658,7 +2615,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B75" s="1">
         <v>44.738218000000003</v>
@@ -2669,7 +2626,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B76" s="1">
         <v>44.727348999999997</v>
@@ -2680,7 +2637,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B77" s="1">
         <v>44.747073999999998</v>
@@ -2691,7 +2648,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B78" s="1">
         <v>44.688110000000002</v>
@@ -2713,7 +2670,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B80" s="1">
         <v>44.660443999999998</v>
@@ -2724,7 +2681,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B81" s="1">
         <v>44.613860000000003</v>
@@ -2746,7 +2703,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B83" s="1">
         <v>44.682794999999999</v>
@@ -2757,7 +2714,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B84" s="1">
         <v>44.668593999999999</v>
@@ -2801,7 +2758,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B88" s="1">
         <v>44.339058999999999</v>
@@ -2823,7 +2780,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B90" s="1">
         <v>44.218671999999998</v>
@@ -2834,7 +2791,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B91" s="1">
         <v>44.164726999999999</v>
@@ -2845,7 +2802,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B92" s="1">
         <v>44.153368999999998</v>
@@ -2867,7 +2824,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B94" s="1">
         <v>45.194276000000002</v>
@@ -2900,7 +2857,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B97" s="1">
         <v>45.554828000000001</v>
@@ -2911,7 +2868,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B98" s="1">
         <v>45.516989000000002</v>
@@ -2944,7 +2901,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B101" s="1">
         <v>45.328017000000003</v>
@@ -2955,7 +2912,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B102" s="1">
         <v>45.229300000000002</v>
@@ -2966,7 +2923,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B103" s="1">
         <v>45.194459999999999</v>
@@ -2977,7 +2934,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B104" s="1">
         <v>45.193187999999999</v>

</xml_diff>

<commit_message>
updates to report, recommendations, site costs based on prioritization mtg notes
</commit_message>
<xml_diff>
--- a/data/prioritization/iptds_site_recommendations_20240411.xlsx
+++ b/data/prioritization/iptds_site_recommendations_20240411.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeRiverIPTDS\data\prioritization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9061891-D011-41A6-A605-451A634B5BD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E5C0ECD-C710-4013-B67E-16DEAC132DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="144">
   <si>
     <t>site_code</t>
   </si>
@@ -402,51 +402,18 @@
     <t>HIGH</t>
   </si>
   <si>
-    <t>Ideally, located below Morgan Creek and above population boundary. Locations near Challis, ID could also be considered.</t>
-  </si>
-  <si>
     <t>Upgrade to IS1001 MC to span river and increase read range.</t>
   </si>
   <si>
-    <t>Upgrade upstream and/or downstream array(s) to FS1001 MUX.</t>
-  </si>
-  <si>
-    <t>If not already, consider upgrade to IS1001 to increase read range.</t>
-  </si>
-  <si>
-    <t>Move to lower boundary of CRSFC-s population.</t>
-  </si>
-  <si>
     <t>Consider decommissioning if LC1 can be converted to a two-pass configuration; alternatively, consider moving upstream to below core spawning areas.</t>
   </si>
   <si>
-    <t>Upgrade to IS1001 MC to increase read range.</t>
-  </si>
-  <si>
     <t>If transfer to IPTDS O&amp;M project is not desired, ensure long-term funding.</t>
   </si>
   <si>
-    <t>Alternative locations: East Fork Salmon River.</t>
-  </si>
-  <si>
-    <t>Alternate locations: upper Chamberlain, Sabe, Bargamin, Warren, Crooked, or Sheep creeks.</t>
-  </si>
-  <si>
-    <t>Alternative locations: Slate Creek, Whitebird Creek.</t>
-  </si>
-  <si>
-    <t>Consider funding either SC3 or SC4 to provide detections to estimate abundance at SC2 at proposed new location.</t>
-  </si>
-  <si>
     <t>Consider upgrade to IS1001 MC and tandem arrays if sufficient distance btw arrays can be achieved.</t>
   </si>
   <si>
-    <t>New site could be a single-pass array.</t>
-  </si>
-  <si>
-    <t>If feasible, SW2 could be moved to the end of the Selway Road which would allow parsing of the SEMOO and SEUMA populations from SEMEA.</t>
-  </si>
-  <si>
     <t>USC (Proposed)</t>
   </si>
   <si>
@@ -459,25 +426,61 @@
     <t>Planned upgrade to IS1001 MC.</t>
   </si>
   <si>
-    <t>Important site for in-season adult monitoring and juvenile survival monitoring.</t>
-  </si>
-  <si>
     <t>WB1 (Proposed)</t>
   </si>
   <si>
-    <t>If not already, consider upgrade to IS1001 MC to increase read range.</t>
-  </si>
-  <si>
-    <t>Move upstream to proposed USP location.</t>
-  </si>
-  <si>
-    <t>One of LAP or (previous) JUL should be funded to provide monitoring in the CRLMA-s population.</t>
+    <t>Upgrade to IS1001 MC to increase read range and improve reliability.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ideally, located below Morgan Creek and above population boundary. Alternately, a location near Challis, ID could be considered. If installed at the proposed location(s), could be a single array. Depending on feasibility of the proposed USC and/or EFS location(s), alternate configurations could be considered. </t>
+  </si>
+  <si>
+    <t>Preference to be installed on the mainstem Upper Salmon River above the SRUMA-s population boundary. If installed at the proposed location, could be a single array. If not feasible, an alternate location would be the lower East Fork Salmon River, but if so, should be a tandem array. Depending on feasibility of the proposed USP location, alternate configurations could be considered.</t>
+  </si>
+  <si>
+    <t>Any remaining infrastructure could be relocated to proposed USC, EFS, and/or USP locations.</t>
+  </si>
+  <si>
+    <t>Long-term, consider upgrades to IS1001 MC to span river and increase read range.</t>
+  </si>
+  <si>
+    <t>Alternate locations: upper Chamberlain, Sabe, Bargamin, Warren, Crooked, or Sheep creeks. Any of the proposed locations would need to be a tandem array.</t>
+  </si>
+  <si>
+    <t>Important site for in-season adult monitoring and juvenile survival monitoring. If transferred from Project, explore other funding sources.</t>
+  </si>
+  <si>
+    <t>Needs to remain tandem site. Downstream array candidate for upgrade to FS1001 MUX.</t>
+  </si>
+  <si>
+    <t>Alternative locations: Slate Creek, Whitebird Creek. At any of the proposed locations, would need to be a tandem array.</t>
+  </si>
+  <si>
+    <t>If desirable, SW2 could be moved to the end of the Selway Road which would allow parsing of the SEMOO and SEUMA Chinook salmon populations from SEMEA.</t>
+  </si>
+  <si>
+    <t>Move to lower boundary of CRSFC-s population. Preferable option would be to install SC2 at new location as a tandem array if arrays could be adequately spaced to ensure independent detections. Alternately, consider funding SC3 or SC4.</t>
+  </si>
+  <si>
+    <t>If SC2 at the proposed site at the population boundary as a tandem array with arrays spaced adequately to ensure independent detections isn't feasible, either SC3 or SC4 should be considered for funding under the project.</t>
+  </si>
+  <si>
+    <t>Consider funding LAP to provide long-term monitoring in the CRLMA-s population.</t>
+  </si>
+  <si>
+    <t>Consider adding remote communications.</t>
+  </si>
+  <si>
+    <t>Upgrade to IS1001 MC to increase read range and improve reliability, especially if IR2 is removed or transferred.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -521,7 +524,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -534,6 +537,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -814,10 +820,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -858,10 +864,10 @@
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="6">
         <v>44.221899999999998</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="6">
         <v>-114.93146</v>
       </c>
       <c r="E2" s="4"/>
@@ -873,37 +879,37 @@
       <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="6">
         <v>44.287737</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="6">
         <v>-114.72045300000001</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>117</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="6">
         <v>44.253700000000002</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="6">
         <v>-114.35290000000001</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>119</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -913,10 +919,10 @@
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="6">
         <v>44.245899999999999</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="6">
         <v>-114.30289999999999</v>
       </c>
       <c r="E5" s="4" t="s">
@@ -925,22 +931,22 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="6">
         <v>44.677300000000002</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="6">
         <v>-114.0744</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>119</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -950,17 +956,17 @@
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="6">
         <v>44.889763000000002</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="6">
         <v>-113.964145</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -970,17 +976,17 @@
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="6">
         <v>45.028530000000003</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="6">
         <v>-113.916319</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>118</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -990,17 +996,17 @@
       <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="6">
         <v>45.176475000000003</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="6">
         <v>-113.885278</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>117</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1010,10 +1016,10 @@
       <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="6">
         <v>45.112189000000001</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="6">
         <v>-113.746897</v>
       </c>
       <c r="E10" s="4" t="s">
@@ -1027,10 +1033,10 @@
       <c r="B11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="6">
         <v>44.861654000000001</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="6">
         <v>-113.63193699999999</v>
       </c>
       <c r="E11" s="4"/>
@@ -1042,15 +1048,15 @@
       <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="6">
         <v>44.865960000000001</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="6">
         <v>-113.62472099999999</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="2" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1060,10 +1066,10 @@
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="6">
         <v>44.780552</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="6">
         <v>-113.545027</v>
       </c>
       <c r="E13" s="4" t="s">
@@ -1077,10 +1083,10 @@
       <c r="B14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="6">
         <v>44.697567999999997</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="6">
         <v>-113.374118</v>
       </c>
       <c r="E14" s="4" t="s">
@@ -1094,10 +1100,10 @@
       <c r="B15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="6">
         <v>44.691090000000003</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="6">
         <v>-113.365281</v>
       </c>
       <c r="E15" s="4" t="s">
@@ -1111,10 +1117,10 @@
       <c r="B16" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="6">
         <v>45.417558</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="6">
         <v>-113.994089</v>
       </c>
       <c r="E16" s="4"/>
@@ -1126,17 +1132,17 @@
       <c r="B17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="6">
         <v>45.295253000000002</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="6">
         <v>-114.358101</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>117</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1146,17 +1152,17 @@
       <c r="B18" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="6">
         <v>45.448700000000002</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="6">
         <v>-114.9449</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>118</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1166,10 +1172,10 @@
       <c r="B19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="6">
         <v>44.408689000000003</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="6">
         <v>-115.179841</v>
       </c>
       <c r="E19" s="4"/>
@@ -1181,10 +1187,10 @@
       <c r="B20" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="6">
         <v>45.103532000000001</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="6">
         <v>-114.85381700000001</v>
       </c>
       <c r="E20" s="4"/>
@@ -1196,17 +1202,17 @@
       <c r="B21" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="6">
         <v>45.175659000000003</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="6">
         <v>-115.579712</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>117</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -1216,10 +1222,10 @@
       <c r="B22" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="6">
         <v>44.978471999999996</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="6">
         <v>-115.726994</v>
       </c>
       <c r="E22" s="4"/>
@@ -1231,17 +1237,17 @@
       <c r="B23" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="6">
         <v>44.956204999999997</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="6">
         <v>-115.53315000000001</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>117</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1251,17 +1257,17 @@
       <c r="B24" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="6">
         <v>45.033299999999997</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="6">
         <v>-115.73302</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>117</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1271,30 +1277,30 @@
       <c r="B25" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="6">
         <v>45.407130000000002</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="6">
         <v>-116.3293</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>119</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="6">
         <v>45.758183000000002</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="6">
         <v>-116.306603</v>
       </c>
       <c r="E26" s="4" t="s">
@@ -1308,10 +1314,10 @@
       <c r="B27" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="6">
         <v>45.639099999999999</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="6">
         <v>-116.2645</v>
       </c>
       <c r="E27" s="4" t="s">
@@ -1325,10 +1331,10 @@
       <c r="B28" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="6">
         <v>46.110317999999999</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="6">
         <v>-115.56588600000001</v>
       </c>
       <c r="E28" s="4" t="s">
@@ -1342,17 +1348,17 @@
       <c r="B29" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="6">
         <v>46.085934000000002</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="6">
         <v>-115.515533</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>119</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1362,10 +1368,10 @@
       <c r="B30" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C30" s="6">
         <v>46.145727000000001</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D30" s="6">
         <v>-115.596497</v>
       </c>
       <c r="E30" s="4"/>
@@ -1377,10 +1383,10 @@
       <c r="B31" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31" s="6">
         <v>46.163820999999999</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D31" s="6">
         <v>-115.589663</v>
       </c>
       <c r="E31" s="4"/>
@@ -1392,18 +1398,13 @@
       <c r="B32" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="6">
         <v>46.137022000000002</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D32" s="6">
         <v>-115.981313</v>
       </c>
-      <c r="E32" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>141</v>
-      </c>
+      <c r="E32" s="4"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
@@ -1412,17 +1413,17 @@
       <c r="B33" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33" s="6">
         <v>46.127209000000001</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D33" s="6">
         <v>-115.97776</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>119</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>124</v>
+        <v>139</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1432,17 +1433,17 @@
       <c r="B34" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="6">
         <v>45.814145000000003</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D34" s="6">
         <v>-115.815972</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>117</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1452,17 +1453,17 @@
       <c r="B35" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C35" s="6">
         <v>45.823500000000003</v>
       </c>
-      <c r="D35" s="3">
+      <c r="D35" s="6">
         <v>-115.6341</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>117</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1470,17 +1471,15 @@
         <v>39</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C36" s="3">
+        <v>5</v>
+      </c>
+      <c r="C36" s="6">
         <v>45.821492999999997</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D36" s="6">
         <v>-115.52766</v>
       </c>
-      <c r="E36" s="4" t="s">
-        <v>117</v>
-      </c>
+      <c r="E36" s="4"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
@@ -1489,17 +1488,17 @@
       <c r="B37" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C37" s="6">
         <v>46.294359999999998</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D37" s="6">
         <v>-115.97615999999999</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>117</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1509,17 +1508,17 @@
       <c r="B38" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C38" s="6">
         <v>46.290497999999999</v>
       </c>
-      <c r="D38" s="3">
+      <c r="D38" s="6">
         <v>-115.933747</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>117</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1529,31 +1528,31 @@
       <c r="B39" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C39" s="3">
+      <c r="C39" s="6">
         <v>46.443272999999998</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D39" s="6">
         <v>-116.812535</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C40" s="3">
-        <v>46.565322999999999</v>
-      </c>
-      <c r="D40" s="3">
-        <v>-116.709318</v>
+        <v>5</v>
+      </c>
+      <c r="C40" s="6">
+        <v>45.761051999999999</v>
+      </c>
+      <c r="D40" s="6">
+        <v>-116.750231</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>118</v>
@@ -1564,66 +1563,65 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" s="3">
-        <v>45.761051999999999</v>
-      </c>
-      <c r="D41" s="3">
-        <v>-116.750231</v>
+        <v>11</v>
+      </c>
+      <c r="C41" s="6">
+        <v>45.742702000000001</v>
+      </c>
+      <c r="D41" s="6">
+        <v>-116.764304</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="3">
-        <v>45.742702000000001</v>
-      </c>
-      <c r="D42" s="3">
-        <v>-116.764304</v>
+      <c r="C42" s="6">
+        <v>45.489956999999997</v>
+      </c>
+      <c r="D42" s="6">
+        <v>-116.804096</v>
       </c>
       <c r="E42" s="4"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C43" s="3">
-        <v>45.489956999999997</v>
-      </c>
-      <c r="D43" s="3">
-        <v>-116.804096</v>
-      </c>
-      <c r="E43" s="4"/>
+        <v>11</v>
+      </c>
+      <c r="C43" s="6">
+        <v>45.767740000000003</v>
+      </c>
+      <c r="D43" s="6">
+        <v>-116.74403700000001</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C44" s="3">
-        <v>45.767740000000003</v>
-      </c>
-      <c r="D44" s="3">
-        <v>-116.74403700000001</v>
+      <c r="C44" s="6">
+        <v>45.506481999999998</v>
+      </c>
+      <c r="D44" s="6">
+        <v>-116.850735</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>117</v>
@@ -1631,151 +1629,134 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C45" s="3">
-        <v>45.506481999999998</v>
-      </c>
-      <c r="D45" s="3">
-        <v>-116.850735</v>
+        <v>5</v>
+      </c>
+      <c r="C45" s="6">
+        <v>45.593519999999998</v>
+      </c>
+      <c r="D45" s="6">
+        <v>-117.903379</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>117</v>
       </c>
+      <c r="F45" s="2" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C46" s="3">
-        <v>45.593519999999998</v>
-      </c>
-      <c r="D46" s="3">
-        <v>-117.903379</v>
+      <c r="C46" s="6">
+        <v>45.633679000000001</v>
+      </c>
+      <c r="D46" s="6">
+        <v>-117.733757</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>118</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C47" s="3">
-        <v>45.633679000000001</v>
-      </c>
-      <c r="D47" s="3">
-        <v>-117.733757</v>
+        <v>7</v>
+      </c>
+      <c r="C47" s="6">
+        <v>45.594465999999997</v>
+      </c>
+      <c r="D47" s="6">
+        <v>-117.579223</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C48" s="3">
-        <v>45.594465999999997</v>
-      </c>
-      <c r="D48" s="3">
-        <v>-117.579223</v>
+      <c r="C48" s="6">
+        <v>45.619622999999997</v>
+      </c>
+      <c r="D48" s="6">
+        <v>-117.72657</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>117</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C49" s="3">
-        <v>45.619622999999997</v>
-      </c>
-      <c r="D49" s="3">
-        <v>-117.72657</v>
+      <c r="C49" s="6">
+        <v>45.946151</v>
+      </c>
+      <c r="D49" s="6">
+        <v>-117.45412399999999</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C50" s="3">
-        <v>45.946151</v>
-      </c>
-      <c r="D50" s="3">
-        <v>-117.45412399999999</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>127</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C50" s="6">
+        <v>46.030237</v>
+      </c>
+      <c r="D50" s="6">
+        <v>-117.016408</v>
+      </c>
+      <c r="E50" s="4"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C51" s="3">
-        <v>46.030237</v>
-      </c>
-      <c r="D51" s="3">
-        <v>-117.016408</v>
-      </c>
-      <c r="E51" s="4"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B52" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C52" s="3">
+      <c r="C51" s="6">
         <v>46.341368000000003</v>
       </c>
-      <c r="D52" s="3">
+      <c r="D51" s="6">
         <v>-117.055707</v>
       </c>
-      <c r="E52" s="4" t="s">
+      <c r="E51" s="4" t="s">
         <v>117</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>